<commit_message>
menambahkan file dinamisKankerParuParu untuk frame input data dinamis
</commit_message>
<xml_diff>
--- a/Data/Perhitungan.xlsx
+++ b/Data/Perhitungan.xlsx
@@ -378,18 +378,23 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -399,7 +404,13 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -411,17 +422,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,6 +437,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -699,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D5:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView tabSelected="1" topLeftCell="D48" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -766,10 +770,10 @@
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="4:15">
-      <c r="D8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8"/>
+      <c r="D8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14"/>
       <c r="F8" s="3" t="s">
         <v>2</v>
       </c>
@@ -947,10 +951,10 @@
       <c r="F17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="4:9">
       <c r="D18" s="3" t="s">
@@ -960,14 +964,14 @@
         <v>3</v>
       </c>
       <c r="F18" s="6">
-        <f>(E18/$E$31)</f>
+        <f t="shared" ref="F18:F30" si="0">(E18/$E$31)</f>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="18">
         <f>(F18*G9)</f>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H18" s="19"/>
+      <c r="H18" s="18"/>
       <c r="I18" t="s">
         <v>4</v>
       </c>
@@ -980,14 +984,14 @@
         <v>1</v>
       </c>
       <c r="F19" s="6">
-        <f>(E19/$E$31)</f>
+        <f t="shared" si="0"/>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="18">
         <f>(F19*G10)</f>
         <v>-2.9411764705882353E-2</v>
       </c>
-      <c r="H19" s="19"/>
+      <c r="H19" s="18"/>
       <c r="I19" t="s">
         <v>6</v>
       </c>
@@ -1000,14 +1004,14 @@
         <v>3</v>
       </c>
       <c r="F20" s="6">
-        <f>(E20/$E$31)</f>
+        <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="18">
         <f>(F20*G11)</f>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H20" s="19"/>
+      <c r="H20" s="18"/>
       <c r="I20" t="s">
         <v>7</v>
       </c>
@@ -1020,14 +1024,14 @@
         <v>4</v>
       </c>
       <c r="F21" s="6">
-        <f>(E21/$E$31)</f>
+        <f t="shared" si="0"/>
         <v>0.11764705882352941</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="18">
         <f>(F21*G12)</f>
         <v>0.11764705882352941</v>
       </c>
-      <c r="H21" s="19"/>
+      <c r="H21" s="18"/>
       <c r="I21" t="s">
         <v>8</v>
       </c>
@@ -1040,14 +1044,14 @@
         <v>2</v>
       </c>
       <c r="F22" s="6">
-        <f>(E22/$E$31)</f>
+        <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="18">
         <f>(F22*G12)</f>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="H22" s="19"/>
+      <c r="H22" s="18"/>
       <c r="I22" t="s">
         <v>10</v>
       </c>
@@ -1060,14 +1064,14 @@
         <v>5</v>
       </c>
       <c r="F23" s="6">
-        <f>(E23/$E$31)</f>
+        <f t="shared" si="0"/>
         <v>0.14705882352941177</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="19">
         <f>F23*1</f>
         <v>0.14705882352941177</v>
       </c>
-      <c r="H23" s="21"/>
+      <c r="H23" s="20"/>
       <c r="I23" t="s">
         <v>33</v>
       </c>
@@ -1080,14 +1084,14 @@
         <v>2</v>
       </c>
       <c r="F24" s="6">
-        <f>(E24/$E$31)</f>
+        <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="G24" s="20">
-        <f t="shared" ref="G24:G30" si="0">F24*1</f>
+      <c r="G24" s="19">
+        <f t="shared" ref="G24:G30" si="1">F24*1</f>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="20"/>
       <c r="I24" t="s">
         <v>34</v>
       </c>
@@ -1100,14 +1104,14 @@
         <v>3</v>
       </c>
       <c r="F25" s="6">
-        <f>(E25/$E$31)</f>
-        <v>8.8235294117647065E-2</v>
-      </c>
-      <c r="G25" s="20">
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H25" s="21"/>
+      <c r="G25" s="19">
+        <f t="shared" si="1"/>
+        <v>8.8235294117647065E-2</v>
+      </c>
+      <c r="H25" s="20"/>
       <c r="I25" t="s">
         <v>35</v>
       </c>
@@ -1120,14 +1124,14 @@
         <v>2</v>
       </c>
       <c r="F26" s="6">
-        <f>(E26/$E$31)</f>
-        <v>5.8823529411764705E-2</v>
-      </c>
-      <c r="G26" s="20">
         <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="H26" s="21"/>
+      <c r="G26" s="19">
+        <f t="shared" si="1"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="H26" s="20"/>
       <c r="I26" t="s">
         <v>36</v>
       </c>
@@ -1140,14 +1144,14 @@
         <v>3</v>
       </c>
       <c r="F27" s="6">
-        <f>(E27/$E$31)</f>
-        <v>8.8235294117647065E-2</v>
-      </c>
-      <c r="G27" s="20">
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H27" s="21"/>
+      <c r="G27" s="19">
+        <f t="shared" si="1"/>
+        <v>8.8235294117647065E-2</v>
+      </c>
+      <c r="H27" s="20"/>
       <c r="I27" t="s">
         <v>37</v>
       </c>
@@ -1160,14 +1164,14 @@
         <v>1</v>
       </c>
       <c r="F28" s="6">
-        <f>(E28/$E$31)</f>
+        <f t="shared" si="0"/>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="G28" s="20">
+      <c r="G28" s="19">
         <f>F28*1</f>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="H28" s="21"/>
+      <c r="H28" s="20"/>
       <c r="I28" t="s">
         <v>38</v>
       </c>
@@ -1180,14 +1184,14 @@
         <v>2</v>
       </c>
       <c r="F29" s="6">
-        <f>(E29/$E$31)</f>
-        <v>5.8823529411764705E-2</v>
-      </c>
-      <c r="G29" s="20">
         <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="H29" s="21"/>
+      <c r="G29" s="19">
+        <f t="shared" si="1"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="H29" s="20"/>
       <c r="I29" t="s">
         <v>39</v>
       </c>
@@ -1200,14 +1204,14 @@
         <v>3</v>
       </c>
       <c r="F30" s="6">
-        <f>(E30/$E$31)</f>
-        <v>8.8235294117647065E-2</v>
-      </c>
-      <c r="G30" s="20">
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="H30" s="21"/>
+      <c r="G30" s="19">
+        <f t="shared" si="1"/>
+        <v>8.8235294117647065E-2</v>
+      </c>
+      <c r="H30" s="20"/>
       <c r="I30" t="s">
         <v>40</v>
       </c>
@@ -1231,19 +1235,19 @@
       </c>
     </row>
     <row r="35" spans="4:17">
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="E35" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
     </row>
     <row r="36" spans="4:17">
-      <c r="D36" s="8"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="2" t="s">
         <v>4</v>
       </c>
@@ -1288,43 +1292,43 @@
       <c r="D37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="22">
+      <c r="E37" s="8">
         <v>33</v>
       </c>
-      <c r="F37" s="22">
-        <v>1</v>
-      </c>
-      <c r="G37" s="22">
+      <c r="F37" s="8">
+        <v>1</v>
+      </c>
+      <c r="G37" s="8">
         <v>4</v>
       </c>
-      <c r="H37" s="22">
+      <c r="H37" s="8">
         <v>5</v>
       </c>
-      <c r="I37" s="22">
+      <c r="I37" s="8">
         <v>4</v>
       </c>
-      <c r="J37" s="22">
+      <c r="J37" s="8">
         <v>3</v>
       </c>
-      <c r="K37" s="22">
+      <c r="K37" s="8">
         <v>2</v>
       </c>
-      <c r="L37" s="22">
+      <c r="L37" s="8">
         <v>4</v>
       </c>
-      <c r="M37" s="22">
+      <c r="M37" s="8">
         <v>3</v>
       </c>
-      <c r="N37" s="22">
+      <c r="N37" s="8">
         <v>2</v>
       </c>
-      <c r="O37" s="22">
+      <c r="O37" s="8">
         <v>3</v>
       </c>
-      <c r="P37" s="22">
+      <c r="P37" s="8">
         <v>2</v>
       </c>
-      <c r="Q37" s="22">
+      <c r="Q37" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1332,43 +1336,43 @@
       <c r="D38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="22">
+      <c r="E38" s="8">
         <v>17</v>
       </c>
-      <c r="F38" s="22">
-        <v>1</v>
-      </c>
-      <c r="G38" s="22">
-        <v>1</v>
-      </c>
-      <c r="H38" s="22">
+      <c r="F38" s="8">
+        <v>1</v>
+      </c>
+      <c r="G38" s="8">
+        <v>1</v>
+      </c>
+      <c r="H38" s="8">
         <v>5</v>
       </c>
-      <c r="I38" s="22">
+      <c r="I38" s="8">
         <v>2</v>
       </c>
-      <c r="J38" s="22">
+      <c r="J38" s="8">
         <v>2</v>
       </c>
-      <c r="K38" s="22">
+      <c r="K38" s="8">
         <v>2</v>
       </c>
-      <c r="L38" s="22">
+      <c r="L38" s="8">
         <v>3</v>
       </c>
-      <c r="M38" s="22">
-        <v>1</v>
-      </c>
-      <c r="N38" s="22">
+      <c r="M38" s="8">
+        <v>1</v>
+      </c>
+      <c r="N38" s="8">
         <v>7</v>
       </c>
-      <c r="O38" s="22">
+      <c r="O38" s="8">
         <v>6</v>
       </c>
-      <c r="P38" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q38" s="22">
+      <c r="P38" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="8">
         <v>7</v>
       </c>
     </row>
@@ -1376,43 +1380,43 @@
       <c r="D39" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="22">
+      <c r="E39" s="8">
         <v>35</v>
       </c>
-      <c r="F39" s="22">
-        <v>1</v>
-      </c>
-      <c r="G39" s="22">
+      <c r="F39" s="8">
+        <v>1</v>
+      </c>
+      <c r="G39" s="8">
         <v>5</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="8">
         <v>6</v>
       </c>
-      <c r="I39" s="22">
+      <c r="I39" s="8">
         <v>7</v>
       </c>
-      <c r="J39" s="22">
+      <c r="J39" s="8">
         <v>2</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K39" s="8">
         <v>4</v>
       </c>
-      <c r="L39" s="22">
+      <c r="L39" s="8">
         <v>8</v>
       </c>
-      <c r="M39" s="22">
+      <c r="M39" s="8">
         <v>8</v>
       </c>
-      <c r="N39" s="22">
+      <c r="N39" s="8">
         <v>9</v>
       </c>
-      <c r="O39" s="22">
-        <v>1</v>
-      </c>
-      <c r="P39" s="22">
+      <c r="O39" s="8">
+        <v>1</v>
+      </c>
+      <c r="P39" s="8">
         <v>6</v>
       </c>
-      <c r="Q39" s="22">
+      <c r="Q39" s="8">
         <v>7</v>
       </c>
     </row>
@@ -1420,43 +1424,43 @@
       <c r="D40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="22">
+      <c r="E40" s="8">
         <v>37</v>
       </c>
-      <c r="F40" s="22">
-        <v>1</v>
-      </c>
-      <c r="G40" s="22">
+      <c r="F40" s="8">
+        <v>1</v>
+      </c>
+      <c r="G40" s="8">
         <v>7</v>
       </c>
-      <c r="H40" s="22">
+      <c r="H40" s="8">
         <v>7</v>
       </c>
-      <c r="I40" s="22">
+      <c r="I40" s="8">
         <v>7</v>
       </c>
-      <c r="J40" s="22">
+      <c r="J40" s="8">
         <v>7</v>
       </c>
-      <c r="K40" s="22">
+      <c r="K40" s="8">
         <v>7</v>
       </c>
-      <c r="L40" s="22">
+      <c r="L40" s="8">
         <v>8</v>
       </c>
-      <c r="M40" s="22">
+      <c r="M40" s="8">
         <v>4</v>
       </c>
-      <c r="N40" s="22">
+      <c r="N40" s="8">
         <v>3</v>
       </c>
-      <c r="O40" s="22">
+      <c r="O40" s="8">
         <v>4</v>
       </c>
-      <c r="P40" s="22">
+      <c r="P40" s="8">
         <v>6</v>
       </c>
-      <c r="Q40" s="22">
+      <c r="Q40" s="8">
         <v>7</v>
       </c>
     </row>
@@ -1467,19 +1471,19 @@
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="4:17">
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="E44" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
     </row>
     <row r="45" spans="4:17">
-      <c r="D45" s="8"/>
+      <c r="D45" s="14"/>
       <c r="E45" s="2" t="s">
         <v>4</v>
       </c>
@@ -1524,55 +1528,55 @@
       <c r="D46" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="23">
+      <c r="E46" s="9">
         <f>E37^0.09</f>
         <v>1.3698286794608083</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="9">
         <f>F37^G19</f>
         <v>1</v>
       </c>
-      <c r="G46" s="23">
+      <c r="G46" s="9">
         <f>G37^0.09</f>
         <v>1.1328838852957985</v>
       </c>
-      <c r="H46" s="23">
+      <c r="H46" s="9">
         <f>H37^0.12</f>
         <v>1.2130435711726304</v>
       </c>
-      <c r="I46" s="23">
+      <c r="I46" s="9">
         <f>I37^0.06</f>
         <v>1.086734862526058</v>
       </c>
-      <c r="J46" s="23">
+      <c r="J46" s="9">
         <f>J37^0.15</f>
         <v>1.1791476456813665</v>
       </c>
-      <c r="K46" s="23">
+      <c r="K46" s="9">
         <f>K37^0.06</f>
         <v>1.0424657608411214</v>
       </c>
-      <c r="L46" s="23">
+      <c r="L46" s="9">
         <f>L37^0.09</f>
         <v>1.1328838852957985</v>
       </c>
-      <c r="M46" s="23">
+      <c r="M46" s="9">
         <f>M37^0.06</f>
         <v>1.068137777449498</v>
       </c>
-      <c r="N46" s="23">
+      <c r="N46" s="9">
         <f>N37^0.09</f>
         <v>1.0643701824533598</v>
       </c>
-      <c r="O46" s="23">
+      <c r="O46" s="9">
         <f>O37^0.03</f>
         <v>1.0335075120430901</v>
       </c>
-      <c r="P46" s="23">
+      <c r="P46" s="9">
         <f>P37^0.06</f>
         <v>1.0424657608411214</v>
       </c>
-      <c r="Q46" s="23">
+      <c r="Q46" s="9">
         <f>Q37^0.09</f>
         <v>1.1039284168910664</v>
       </c>
@@ -1581,56 +1585,56 @@
       <c r="D47" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E47" s="9">
         <f>E38^0.09</f>
         <v>1.2904476852080027</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="9">
         <f>F38^G19</f>
         <v>1</v>
       </c>
-      <c r="G47" s="23">
+      <c r="G47" s="9">
         <f>G38^0.09</f>
         <v>1</v>
       </c>
-      <c r="H47" s="23">
-        <f t="shared" ref="H47:H49" si="1">H38^0.12</f>
+      <c r="H47" s="9">
+        <f t="shared" ref="H47:H49" si="2">H38^0.12</f>
         <v>1.2130435711726304</v>
       </c>
-      <c r="I47" s="23">
-        <f t="shared" ref="I47:I49" si="2">I38^0.06</f>
+      <c r="I47" s="9">
+        <f t="shared" ref="I47:I49" si="3">I38^0.06</f>
         <v>1.0424657608411214</v>
       </c>
-      <c r="J47" s="23">
-        <f t="shared" ref="J47:J49" si="3">J38^0.15</f>
+      <c r="J47" s="9">
+        <f t="shared" ref="J47:J49" si="4">J38^0.15</f>
         <v>1.1095694720678451</v>
       </c>
-      <c r="K47" s="23">
-        <f t="shared" ref="K47:K49" si="4">K38^0.06</f>
+      <c r="K47" s="9">
+        <f t="shared" ref="K47:K49" si="5">K38^0.06</f>
         <v>1.0424657608411214</v>
       </c>
-      <c r="L47" s="23">
-        <f t="shared" ref="L47:L49" si="5">L38^0.09</f>
+      <c r="L47" s="9">
+        <f t="shared" ref="L47:L49" si="6">L38^0.09</f>
         <v>1.1039284168910664</v>
       </c>
-      <c r="M47" s="23">
-        <f t="shared" ref="M47:M49" si="6">M38^0.06</f>
-        <v>1</v>
-      </c>
-      <c r="N47" s="23">
-        <f t="shared" ref="N47:N49" si="7">N38^0.09</f>
+      <c r="M47" s="9">
+        <f t="shared" ref="M47:M49" si="7">M38^0.06</f>
+        <v>1</v>
+      </c>
+      <c r="N47" s="9">
+        <f t="shared" ref="N47:N49" si="8">N38^0.09</f>
         <v>1.1914033683338536</v>
       </c>
-      <c r="O47" s="23">
-        <f t="shared" ref="O47:O49" si="8">O38^0.03</f>
+      <c r="O47" s="9">
+        <f t="shared" ref="O47:O49" si="9">O38^0.03</f>
         <v>1.055223701805468</v>
       </c>
-      <c r="P47" s="23">
-        <f t="shared" ref="P47:P49" si="9">P38^0.06</f>
-        <v>1</v>
-      </c>
-      <c r="Q47" s="23">
-        <f t="shared" ref="Q47:Q49" si="10">Q38^0.09</f>
+      <c r="P47" s="9">
+        <f t="shared" ref="P47:P49" si="10">P38^0.06</f>
+        <v>1</v>
+      </c>
+      <c r="Q47" s="9">
+        <f t="shared" ref="Q47:Q49" si="11">Q38^0.09</f>
         <v>1.1914033683338536</v>
       </c>
     </row>
@@ -1638,56 +1642,56 @@
       <c r="D48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="23">
+      <c r="E48" s="9">
         <f>E39^0.09</f>
         <v>1.3771020474505347</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F48" s="9">
         <f>F39^G19</f>
         <v>1</v>
       </c>
-      <c r="G48" s="23">
+      <c r="G48" s="9">
         <f>G39^0.09</f>
         <v>1.1558654978257916</v>
       </c>
-      <c r="H48" s="23">
-        <f t="shared" si="1"/>
+      <c r="H48" s="9">
+        <f t="shared" si="2"/>
         <v>1.2398757045261211</v>
       </c>
-      <c r="I48" s="23">
-        <f t="shared" si="2"/>
+      <c r="I48" s="9">
+        <f t="shared" si="3"/>
         <v>1.1238436146785018</v>
       </c>
-      <c r="J48" s="23">
-        <f t="shared" si="3"/>
+      <c r="J48" s="9">
+        <f t="shared" si="4"/>
         <v>1.1095694720678451</v>
       </c>
-      <c r="K48" s="23">
-        <f t="shared" si="4"/>
+      <c r="K48" s="9">
+        <f t="shared" si="5"/>
         <v>1.086734862526058</v>
       </c>
-      <c r="L48" s="23">
-        <f t="shared" si="5"/>
+      <c r="L48" s="9">
+        <f t="shared" si="6"/>
         <v>1.2058078276907604</v>
       </c>
-      <c r="M48" s="23">
-        <f t="shared" si="6"/>
+      <c r="M48" s="9">
+        <f t="shared" si="7"/>
         <v>1.1328838852957985</v>
       </c>
-      <c r="N48" s="23">
-        <f t="shared" si="7"/>
+      <c r="N48" s="9">
+        <f t="shared" si="8"/>
         <v>1.2186579496196162</v>
       </c>
-      <c r="O48" s="23">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="P48" s="23">
+      <c r="O48" s="9">
         <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="P48" s="9">
+        <f t="shared" si="10"/>
         <v>1.1134970608520351</v>
       </c>
-      <c r="Q48" s="23">
-        <f t="shared" si="10"/>
+      <c r="Q48" s="9">
+        <f t="shared" si="11"/>
         <v>1.1914033683338536</v>
       </c>
     </row>
@@ -1695,56 +1699,56 @@
       <c r="D49" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="23">
+      <c r="E49" s="9">
         <f>E40^0.09</f>
         <v>1.3840065808560691</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F49" s="9">
         <f>F40^G19</f>
         <v>1</v>
       </c>
-      <c r="G49" s="23">
+      <c r="G49" s="9">
         <f>G40^0.09</f>
         <v>1.1914033683338536</v>
       </c>
-      <c r="H49" s="23">
-        <f t="shared" si="1"/>
+      <c r="H49" s="9">
+        <f t="shared" si="2"/>
         <v>1.2630244702536411</v>
       </c>
-      <c r="I49" s="23">
-        <f t="shared" si="2"/>
+      <c r="I49" s="9">
+        <f t="shared" si="3"/>
         <v>1.1238436146785018</v>
       </c>
-      <c r="J49" s="23">
-        <f t="shared" si="3"/>
+      <c r="J49" s="9">
+        <f t="shared" si="4"/>
         <v>1.3389510680084606</v>
       </c>
-      <c r="K49" s="23">
-        <f t="shared" si="4"/>
+      <c r="K49" s="9">
+        <f t="shared" si="5"/>
         <v>1.1238436146785018</v>
       </c>
-      <c r="L49" s="23">
-        <f t="shared" si="5"/>
+      <c r="L49" s="9">
+        <f t="shared" si="6"/>
         <v>1.2058078276907604</v>
       </c>
-      <c r="M49" s="23">
-        <f t="shared" si="6"/>
+      <c r="M49" s="9">
+        <f t="shared" si="7"/>
         <v>1.086734862526058</v>
       </c>
-      <c r="N49" s="23">
-        <f t="shared" si="7"/>
+      <c r="N49" s="9">
+        <f t="shared" si="8"/>
         <v>1.1039284168910664</v>
       </c>
-      <c r="O49" s="23">
-        <f t="shared" si="8"/>
+      <c r="O49" s="9">
+        <f t="shared" si="9"/>
         <v>1.0424657608411214</v>
       </c>
-      <c r="P49" s="23">
-        <f t="shared" si="9"/>
+      <c r="P49" s="9">
+        <f t="shared" si="10"/>
         <v>1.1134970608520351</v>
       </c>
-      <c r="Q49" s="23">
-        <f t="shared" si="10"/>
+      <c r="Q49" s="9">
+        <f t="shared" si="11"/>
         <v>1.1914033683338536</v>
       </c>
     </row>
@@ -1753,55 +1757,55 @@
       <c r="E50" s="1"/>
     </row>
     <row r="52" spans="4:17">
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="15" t="s">
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K52" s="15"/>
-      <c r="L52" s="9" t="s">
+      <c r="K52" s="10"/>
+      <c r="L52" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O52" s="15" t="s">
+      <c r="O52" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="9" t="s">
+      <c r="P52" s="10"/>
+      <c r="Q52" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="53" spans="4:17">
-      <c r="D53" s="15"/>
-      <c r="E53" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="8" t="s">
+      <c r="D53" s="10"/>
+      <c r="E53" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K53" s="8" t="s">
+      <c r="K53" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="L53" s="10"/>
-      <c r="O53" s="8" t="s">
+      <c r="L53" s="12"/>
+      <c r="O53" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="P53" s="8" t="s">
+      <c r="P53" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="Q53" s="10"/>
+      <c r="Q53" s="12"/>
     </row>
     <row r="54" spans="4:17">
-      <c r="D54" s="15"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="2" t="s">
         <v>4</v>
       </c>
@@ -1817,12 +1821,12 @@
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="11"/>
-      <c r="O54" s="8"/>
-      <c r="P54" s="8"/>
-      <c r="Q54" s="11"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="13"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="13"/>
     </row>
     <row r="55" spans="4:17">
       <c r="D55" s="2" t="s">
@@ -1856,7 +1860,7 @@
         <f>(J55/$J$59)</f>
         <v>0.34656164615910373</v>
       </c>
-      <c r="L55" s="12">
+      <c r="L55" s="15">
         <f>MAX(K55:K57)</f>
         <v>0.38136965126321654</v>
       </c>
@@ -1868,7 +1872,7 @@
         <f>O55/O59</f>
         <v>0.19332695223357704</v>
       </c>
-      <c r="Q55" s="12">
+      <c r="Q55" s="15">
         <f>MAX(P55:P58)</f>
         <v>0.35361164794916272</v>
       </c>
@@ -1905,16 +1909,16 @@
         <f>(J56/$J$59)</f>
         <v>0.27206870257767968</v>
       </c>
-      <c r="L56" s="13"/>
+      <c r="L56" s="16"/>
       <c r="O56" s="6">
-        <f t="shared" ref="O56:O58" si="11">E47*F47*G47*H47*I47*J47*K47*L47*M47*N47*O47*P47*Q47</f>
+        <f t="shared" ref="O56:O58" si="12">E47*F47*G47*H47*I47*J47*K47*L47*M47*N47*O47*P47*Q47</f>
         <v>3.1210304074475959</v>
       </c>
       <c r="P56" s="7">
         <f>O56/O59</f>
         <v>0.15663436044771598</v>
       </c>
-      <c r="Q56" s="13"/>
+      <c r="Q56" s="16"/>
     </row>
     <row r="57" spans="4:17">
       <c r="D57" s="2" t="s">
@@ -1948,16 +1952,16 @@
         <f>(J57/$J$59)</f>
         <v>0.38136965126321654</v>
       </c>
-      <c r="L57" s="13"/>
+      <c r="L57" s="16"/>
       <c r="O57" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.9064805501014463</v>
       </c>
       <c r="P57" s="7">
         <f>O57/O59</f>
         <v>0.2964270393695444</v>
       </c>
-      <c r="Q57" s="13"/>
+      <c r="Q57" s="16"/>
     </row>
     <row r="58" spans="4:17">
       <c r="D58" s="4"/>
@@ -1968,26 +1972,26 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="14"/>
+      <c r="L58" s="17"/>
       <c r="O58" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.0459170166904723</v>
       </c>
       <c r="P58" s="7">
         <f>O58/O59</f>
         <v>0.35361164794916272</v>
       </c>
-      <c r="Q58" s="14"/>
+      <c r="Q58" s="17"/>
     </row>
     <row r="59" spans="4:17">
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="18"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="23"/>
       <c r="J59" s="6">
         <f>SUM(J55:J57)</f>
         <v>6.0629456108620143</v>
@@ -2003,19 +2007,10 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="O52:P52"/>
-    <mergeCell ref="Q52:Q54"/>
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="P53:P54"/>
-    <mergeCell ref="Q55:Q58"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="L52:L54"/>
+    <mergeCell ref="L55:L58"/>
+    <mergeCell ref="E53:I53"/>
+    <mergeCell ref="D59:I59"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="J53:J54"/>
@@ -2032,10 +2027,19 @@
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="E44:I44"/>
     <mergeCell ref="K53:K54"/>
-    <mergeCell ref="L52:L54"/>
-    <mergeCell ref="L55:L58"/>
-    <mergeCell ref="E53:I53"/>
-    <mergeCell ref="D59:I59"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="Q52:Q54"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="P53:P54"/>
+    <mergeCell ref="Q55:Q58"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>